<commit_message>
one each add, delete and change
</commit_message>
<xml_diff>
--- a/VT_REG2_TRA_V12.xlsx
+++ b/VT_REG2_TRA_V12.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\ETSAP_DemoS_VFE\DemoS_Adv_Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\testingmodels\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB74487-CAAF-4046-921A-F7999328C557}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9555" yWindow="45" windowWidth="9600" windowHeight="10950" tabRatio="901"/>
+    <workbookView xWindow="-28920" yWindow="-2175" windowWidth="29040" windowHeight="15840" tabRatio="901" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EB2" sheetId="133" r:id="rId1"/>
@@ -26,17 +27,27 @@
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
-    <comment ref="C8" authorId="0" shapeId="0">
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -54,14 +65,14 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gary Goldstein</author>
     <author>Amit Kanudia</author>
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
-    <comment ref="J3" authorId="0" shapeId="0">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -175,7 +186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="1" shapeId="0">
+    <comment ref="O3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -201,7 +212,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="2" shapeId="0">
+    <comment ref="P3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -274,7 +285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="2" shapeId="0">
+    <comment ref="Q3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -327,7 +338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="2" shapeId="0">
+    <comment ref="R3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -360,7 +371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P13" authorId="2" shapeId="0">
+    <comment ref="P13" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -453,7 +464,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q13" authorId="1" shapeId="0">
+    <comment ref="Q13" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
       <text>
         <r>
           <rPr>
@@ -478,7 +489,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R13" authorId="2" shapeId="0">
+    <comment ref="R13" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
       <text>
         <r>
           <rPr>
@@ -541,7 +552,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J14" authorId="2" shapeId="0">
+    <comment ref="J14" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
       <text>
         <r>
           <rPr>
@@ -789,14 +800,14 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gary Goldstein</author>
     <author>Amit Kanudia</author>
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
-    <comment ref="O3" authorId="0" shapeId="0">
+    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -910,7 +921,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="1" shapeId="0">
+    <comment ref="T3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -936,7 +947,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U3" authorId="2" shapeId="0">
+    <comment ref="U3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -1009,7 +1020,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V3" authorId="2" shapeId="0">
+    <comment ref="V3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -1062,7 +1073,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W3" authorId="2" shapeId="0">
+    <comment ref="W3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -1095,7 +1106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U10" authorId="2" shapeId="0">
+    <comment ref="U10" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
       <text>
         <r>
           <rPr>
@@ -1188,7 +1199,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V10" authorId="1" shapeId="0">
+    <comment ref="V10" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
       <text>
         <r>
           <rPr>
@@ -1213,7 +1224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W10" authorId="2" shapeId="0">
+    <comment ref="W10" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
       <text>
         <r>
           <rPr>
@@ -1276,7 +1287,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O11" authorId="2" shapeId="0">
+    <comment ref="O11" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
       <text>
         <r>
           <rPr>
@@ -2066,14 +2077,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="0.000"/>
-    <numFmt numFmtId="179" formatCode="General_)"/>
-    <numFmt numFmtId="187" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="General_)"/>
+    <numFmt numFmtId="167" formatCode="\Te\x\t"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2103,32 +2114,6 @@
       <sz val="10"/>
       <color indexed="12"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -2595,48 +2580,48 @@
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="144">
@@ -2658,33 +2643,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="11" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" xfId="11" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="11" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" xfId="11" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="14" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="27" fillId="0" borderId="0" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="0" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="15"/>
@@ -2701,83 +2686,83 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="15" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="15" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="29" fillId="14" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="25" fillId="14" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" xfId="11" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="5" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" xfId="11" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="179" fontId="13" fillId="17" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="17" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="17" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="23" fillId="11" borderId="0" xfId="12" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="21" fillId="9" borderId="4" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="19" fillId="11" borderId="0" xfId="12" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="17" fillId="9" borderId="4" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="21" fillId="9" borderId="5" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="9" borderId="5" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="179" fontId="21" fillId="9" borderId="6" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="17" fillId="9" borderId="6" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="17" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="17" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="7" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -2788,30 +2773,30 @@
     <xf numFmtId="2" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="13" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="13" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="18" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="3"/>
-    <xf numFmtId="179" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="3"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2819,7 +2804,7 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="3" fillId="17" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="3" fillId="17" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2828,32 +2813,32 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="13" fillId="17" borderId="10" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="9" fillId="17" borderId="10" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="17" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="9" fillId="17" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="17" borderId="11" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="9" fillId="17" borderId="11" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="17" borderId="2" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="9" fillId="17" borderId="2" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="23" fillId="11" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="23" fillId="11" borderId="2" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="19" fillId="11" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="19" fillId="11" borderId="2" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="35" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="29" fillId="14" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="25" fillId="14" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -2866,50 +2851,50 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="15" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="15" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="23" fillId="11" borderId="16" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="23" fillId="11" borderId="14" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="13" fillId="17" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="11" borderId="16" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="19" fillId="11" borderId="14" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="9" fillId="17" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="17" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="17" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="29" fillId="14" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="25" fillId="14" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="29" fillId="14" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="25" fillId="14" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="187" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="187" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="187" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="187" fontId="26" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="22" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="187" fontId="26" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="22" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="187" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="187" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="187" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
@@ -2918,44 +2903,44 @@
     <cellStyle name="Accent1" xfId="4" builtinId="29"/>
     <cellStyle name="Accent2" xfId="5" builtinId="33"/>
     <cellStyle name="Calculation" xfId="6" builtinId="22"/>
-    <cellStyle name="Comma 2" xfId="7"/>
-    <cellStyle name="Comma 2 2" xfId="8"/>
-    <cellStyle name="Comma 2 3" xfId="9"/>
-    <cellStyle name="Comma 2 4" xfId="10"/>
+    <cellStyle name="Comma 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Comma 2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Comma 2 3" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Comma 2 4" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Good" xfId="11" builtinId="26"/>
     <cellStyle name="Input" xfId="12" builtinId="20"/>
-    <cellStyle name="Migliaia_tab emissioni" xfId="13"/>
+    <cellStyle name="Migliaia_tab emissioni" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Neutral" xfId="14" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="15"/>
-    <cellStyle name="Normal 2" xfId="16"/>
-    <cellStyle name="Normal 2 3" xfId="17"/>
-    <cellStyle name="Normal 4" xfId="18"/>
-    <cellStyle name="Normal 4 2" xfId="19"/>
-    <cellStyle name="Normal 8" xfId="20"/>
-    <cellStyle name="Normal 9 2" xfId="21"/>
-    <cellStyle name="Normale_B2020" xfId="22"/>
+    <cellStyle name="Normal 10" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal 2 3" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal 4" xfId="18" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normal 4 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Normal 8" xfId="20" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Normal 9 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Normale_B2020" xfId="22" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
     <cellStyle name="Percent" xfId="23" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="24"/>
-    <cellStyle name="Percent 3" xfId="25"/>
-    <cellStyle name="Percent 3 2" xfId="26"/>
-    <cellStyle name="Percent 3 3" xfId="27"/>
-    <cellStyle name="Percent 3 4" xfId="28"/>
-    <cellStyle name="Percent 3 5" xfId="29"/>
-    <cellStyle name="Percent 4" xfId="30"/>
-    <cellStyle name="Percent 4 2" xfId="31"/>
-    <cellStyle name="Percent 4 3" xfId="32"/>
-    <cellStyle name="Percent 4 4" xfId="33"/>
-    <cellStyle name="Percent 4 5" xfId="34"/>
-    <cellStyle name="Percent 5" xfId="35"/>
-    <cellStyle name="Percent 5 2" xfId="36"/>
-    <cellStyle name="Percent 5 3" xfId="37"/>
-    <cellStyle name="Percent 5 4" xfId="38"/>
-    <cellStyle name="Percent 6" xfId="39"/>
-    <cellStyle name="Percent 7" xfId="40"/>
-    <cellStyle name="Percent 8" xfId="41"/>
-    <cellStyle name="Percent 9" xfId="42"/>
-    <cellStyle name="Standard_Sce_D_Extraction" xfId="43"/>
+    <cellStyle name="Percent 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Percent 3" xfId="25" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Percent 3 2" xfId="26" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Percent 3 3" xfId="27" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Percent 3 4" xfId="28" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Percent 3 5" xfId="29" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Percent 4" xfId="30" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Percent 4 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Percent 4 3" xfId="32" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Percent 4 4" xfId="33" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Percent 4 5" xfId="34" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Percent 5" xfId="35" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Percent 5 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Percent 5 3" xfId="37" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Percent 5 4" xfId="38" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Percent 6" xfId="39" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Percent 7" xfId="40" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Percent 8" xfId="41" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Percent 9" xfId="42" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Standard_Sce_D_Extraction" xfId="43" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2987,7 +2972,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3077,7 +3068,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="57460" name="Picture 6"/>
+        <xdr:cNvPr id="57460" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000074E00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3145,7 +3142,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="57461" name="Picture 8"/>
+        <xdr:cNvPr id="57461" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000075E00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3213,7 +3216,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="57462" name="Picture 4"/>
+        <xdr:cNvPr id="57462" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000076E00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3281,7 +3290,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="57463" name="Picture 5"/>
+        <xdr:cNvPr id="57463" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000077E00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3354,7 +3369,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3507,7 +3528,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3708,7 +3735,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3810,7 +3843,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4832,14 +4871,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:AA31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:U9"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5984,7 +6023,7 @@
       </c>
       <c r="F25" s="102"/>
       <c r="G25" s="105">
-        <v>0.9</v>
+        <v>0.99</v>
       </c>
       <c r="H25" s="102"/>
       <c r="I25" s="105">
@@ -6030,7 +6069,7 @@
       <c r="F26" s="104"/>
       <c r="G26" s="106">
         <f>1-G25</f>
-        <v>9.9999999999999978E-2</v>
+        <v>1.0000000000000009E-2</v>
       </c>
       <c r="H26" s="104"/>
       <c r="I26" s="106">
@@ -6120,7 +6159,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:G5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -6156,7 +6195,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:R36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -7067,7 +7106,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -7572,7 +7611,7 @@
       </c>
       <c r="E14" s="73">
         <f>('EB2'!G$9*'EB2'!$G$25*F14/(K14*G14))*1.01</f>
-        <v>87102.97230272727</v>
+        <v>95813.269532999999</v>
       </c>
       <c r="F14" s="77">
         <v>0.41</v>
@@ -7594,7 +7633,7 @@
       </c>
       <c r="M14" s="39">
         <f t="shared" ref="M14:M22" si="4">E14*G14*K14*H14</f>
-        <v>1796.4988037437502</v>
+        <v>1976.1486841181249</v>
       </c>
       <c r="O14" s="134"/>
       <c r="P14" s="134"/>
@@ -7945,7 +7984,7 @@
       </c>
       <c r="E20" s="73">
         <f>('EB2'!G$9*'EB2'!$G$26*F20/(K20*G20))*1.01</f>
-        <v>1168.4545064999998</v>
+        <v>116.8454506500001</v>
       </c>
       <c r="F20" s="77">
         <v>0.15</v>
@@ -7967,7 +8006,7 @@
       </c>
       <c r="M20" s="39">
         <f>E20*G20*K20*H20</f>
-        <v>876.34087987499981</v>
+        <v>87.634087987500081</v>
       </c>
       <c r="O20" s="134"/>
       <c r="P20" s="134"/>
@@ -8317,7 +8356,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8427,7 +8466,7 @@
       </c>
       <c r="E9" s="72">
         <f>SUM(DemTechs_TRA!M13:M18)</f>
-        <v>3067.06485564375</v>
+        <v>3246.7147360181252</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
@@ -8443,7 +8482,7 @@
       </c>
       <c r="E10" s="72">
         <f>SUM(DemTechs_TRA!M19:M24)</f>
-        <v>1727.9701023749997</v>
+        <v>939.26331048749989</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
@@ -8474,7 +8513,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B3:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
one file delete and editted
</commit_message>
<xml_diff>
--- a/VT_REG2_TRA_V12.xlsx
+++ b/VT_REG2_TRA_V12.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\testingmodels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB74487-CAAF-4046-921A-F7999328C557}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920E8AA1-31B1-4D6D-B15B-0D423000448B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2175" windowWidth="29040" windowHeight="15840" tabRatio="901" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4878,7 +4878,7 @@
   <dimension ref="A1:AA31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6023,7 +6023,7 @@
       </c>
       <c r="F25" s="102"/>
       <c r="G25" s="105">
-        <v>0.99</v>
+        <v>0.9</v>
       </c>
       <c r="H25" s="102"/>
       <c r="I25" s="105">
@@ -6069,7 +6069,7 @@
       <c r="F26" s="104"/>
       <c r="G26" s="106">
         <f>1-G25</f>
-        <v>1.0000000000000009E-2</v>
+        <v>9.9999999999999978E-2</v>
       </c>
       <c r="H26" s="104"/>
       <c r="I26" s="106">
@@ -7611,7 +7611,7 @@
       </c>
       <c r="E14" s="73">
         <f>('EB2'!G$9*'EB2'!$G$25*F14/(K14*G14))*1.01</f>
-        <v>95813.269532999999</v>
+        <v>87102.97230272727</v>
       </c>
       <c r="F14" s="77">
         <v>0.41</v>
@@ -7633,7 +7633,7 @@
       </c>
       <c r="M14" s="39">
         <f t="shared" ref="M14:M22" si="4">E14*G14*K14*H14</f>
-        <v>1976.1486841181249</v>
+        <v>1796.4988037437502</v>
       </c>
       <c r="O14" s="134"/>
       <c r="P14" s="134"/>
@@ -7984,7 +7984,7 @@
       </c>
       <c r="E20" s="73">
         <f>('EB2'!G$9*'EB2'!$G$26*F20/(K20*G20))*1.01</f>
-        <v>116.8454506500001</v>
+        <v>1168.4545064999998</v>
       </c>
       <c r="F20" s="77">
         <v>0.15</v>
@@ -8006,7 +8006,7 @@
       </c>
       <c r="M20" s="39">
         <f>E20*G20*K20*H20</f>
-        <v>87.634087987500081</v>
+        <v>876.34087987499981</v>
       </c>
       <c r="O20" s="134"/>
       <c r="P20" s="134"/>
@@ -8466,7 +8466,7 @@
       </c>
       <c r="E9" s="72">
         <f>SUM(DemTechs_TRA!M13:M18)</f>
-        <v>3246.7147360181252</v>
+        <v>3067.06485564375</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
@@ -8482,7 +8482,7 @@
       </c>
       <c r="E10" s="72">
         <f>SUM(DemTechs_TRA!M19:M24)</f>
-        <v>939.26331048749989</v>
+        <v>1727.9701023749997</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>